<commit_message>
fix bug in ProjectScenario
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Dropbox (UC Berkeley Biostat)/jsLEMMA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D2183D-9ECF-6045-BB73-FCD36A1A1A04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E7E8E-6BCD-C646-9A37-868A4A89E145}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30740" windowHeight="15040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9321,7 +9321,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>